<commit_message>
add more test case for ZSS-241 (ZSS-528)
</commit_message>
<xml_diff>
--- a/zss.test/src/main/webapp/issue/241-wrap.xlsx
+++ b/zss.test/src/main/webapp/issue/241-wrap.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
   <si>
     <t>LooooooooongTextWithoutSpaceOrBreak</t>
   </si>
@@ -30,13 +30,25 @@
     <t>No Wrap</t>
   </si>
   <si>
-    <t>Wrap Text Row</t>
-  </si>
-  <si>
     <t>Merged</t>
   </si>
   <si>
-    <t>High Cell</t>
+    <t>Custom Height</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Initial Wrap Text </t>
+  </si>
+  <si>
+    <t>looooong text</t>
+  </si>
+  <si>
+    <t>veeeeeeeeeeeeeery loooooooooooong text</t>
+  </si>
+  <si>
+    <t>loooooong text</t>
+  </si>
+  <si>
+    <t>Multiple</t>
   </si>
 </sst>
 </file>
@@ -97,74 +109,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -176,7 +120,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="C7EDCC"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -453,28 +397,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:C7"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="75">
+    <row r="1" spans="1:4" ht="75">
       <c r="A1" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="75">
+    <row r="2" spans="1:4" ht="75">
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:4">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -482,40 +429,54 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:4">
       <c r="B4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="17.25" customHeight="1">
+    <row r="5" spans="1:4" ht="17.25" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C5" s="4"/>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:4">
       <c r="B6" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="4"/>
     </row>
-    <row r="7" spans="1:3" ht="69.75" customHeight="1">
-      <c r="A7" s="3" t="s">
-        <v>6</v>
+    <row r="7" spans="1:4" ht="69.75" customHeight="1">
+      <c r="A7" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C7" s="4"/>
     </row>
-    <row r="8" spans="1:3" ht="64.5" customHeight="1">
+    <row r="8" spans="1:4" ht="64.5" customHeight="1">
       <c r="B8" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C8" s="4"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
add more test cases for ZSS-241 (ZSS-528)
</commit_message>
<xml_diff>
--- a/zss.test/src/main/webapp/issue/241-wrap.xlsx
+++ b/zss.test/src/main/webapp/issue/241-wrap.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
   <si>
     <t>LooooooooongTextWithoutSpaceOrBreak</t>
   </si>
@@ -30,13 +30,25 @@
     <t>No Wrap</t>
   </si>
   <si>
-    <t>Wrap Text Row</t>
-  </si>
-  <si>
     <t>Merged</t>
   </si>
   <si>
-    <t>High Cell</t>
+    <t>Custom Height</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Initial Wrap Text </t>
+  </si>
+  <si>
+    <t>looooong text</t>
+  </si>
+  <si>
+    <t>veeeeeeeeeeeeeery loooooooooooong text</t>
+  </si>
+  <si>
+    <t>loooooong text</t>
+  </si>
+  <si>
+    <t>Multiple</t>
   </si>
 </sst>
 </file>
@@ -97,74 +109,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -176,7 +120,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="C7EDCC"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -453,28 +397,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:C7"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="75">
+    <row r="1" spans="1:4" ht="75">
       <c r="A1" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="75">
+    <row r="2" spans="1:4" ht="75">
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:4">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -482,40 +429,54 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:4">
       <c r="B4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="17.25" customHeight="1">
+    <row r="5" spans="1:4" ht="17.25" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C5" s="4"/>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:4">
       <c r="B6" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="4"/>
     </row>
-    <row r="7" spans="1:3" ht="69.75" customHeight="1">
-      <c r="A7" s="3" t="s">
-        <v>6</v>
+    <row r="7" spans="1:4" ht="69.75" customHeight="1">
+      <c r="A7" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C7" s="4"/>
     </row>
-    <row r="8" spans="1:3" ht="64.5" customHeight="1">
+    <row r="8" spans="1:4" ht="64.5" customHeight="1">
       <c r="B8" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C8" s="4"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>